<commit_message>
Atualização de Diagrama Entidade-Relacionamento para Modelo Entidade-Relacionamento
</commit_message>
<xml_diff>
--- a/Gráfico de Gantt.xlsx
+++ b/Gráfico de Gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danilo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danilo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FCFBEB-ABF8-487B-86AA-C3C8E69BB7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEF5660-8459-49FA-84B7-22BD687FF6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0F388947-D0E9-48D2-A0AF-30747250EBEE}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Requisitos e Regras de Negócios</t>
   </si>
   <si>
-    <t>Diagrama de Classe e Diagrama de Entidade e Relacionamento</t>
-  </si>
-  <si>
     <t>Diagrama de Caso de Uso e Especificação</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>Duração (dias)</t>
+  </si>
+  <si>
+    <t>Diagrama de Classe e Modelo Entidade-Relacionamento</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
                   <c:v>Desenvolvimento de Funcionalidades do Sistema</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Diagrama de Classe e Diagrama de Entidade e Relacionamento</c:v>
+                  <c:v>Diagrama de Classe e Modelo Entidade-Relacionamento</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Entrega Final</c:v>
@@ -425,7 +425,7 @@
                   <c:v>Desenvolvimento de Funcionalidades do Sistema</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Diagrama de Classe e Diagrama de Entidade e Relacionamento</c:v>
+                  <c:v>Diagrama de Classe e Modelo Entidade-Relacionamento</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Entrega Final</c:v>
@@ -1563,7 +1563,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9">
         <v>44809</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="9">
         <v>44816</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="9">
         <v>44823</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="9">
         <v>44830</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="9">
         <v>44837</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="9">
         <v>44837</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B9" s="9">
         <v>44851</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="12">
         <v>44872</v>

</xml_diff>